<commit_message>
Individual reports for each test suite
</commit_message>
<xml_diff>
--- a/src/main/java/com/ebay/automation/testdata/TestData_EBayAutomation.xlsx
+++ b/src/main/java/com/ebay/automation/testdata/TestData_EBayAutomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aparn\eclipse-workspace\EBayAutomation\src\main\java\com\ebay\automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ECF5C4-D027-4707-9B8F-F3B00ED0F8B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9DE1A0-2D0F-4A06-8C46-34E9FBE39AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
-  <si>
-    <t>Password;harekrsna88</t>
-  </si>
-  <si>
-    <t>EmaidId;aparna12.rao@gmail.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Electronics, Cars, Fashion, Collectibles &amp; More | eBay</t>
   </si>
@@ -49,21 +43,12 @@
     <t>ExpectedResultsCount</t>
   </si>
   <si>
-    <t>Manjunath</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
     <t>LastName</t>
   </si>
   <si>
-    <t>KV</t>
-  </si>
-  <si>
-    <t>kvm.nath123@gmail.com</t>
-  </si>
-  <si>
     <t>RegisterEmailId</t>
   </si>
   <si>
@@ -89,6 +74,18 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Sriram</t>
+  </si>
+  <si>
+    <t>Rao</t>
+  </si>
+  <si>
+    <t>srirammurthyrao@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -153,13 +150,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +442,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,74 +461,74 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>20</v>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +542,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,18 +553,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>